<commit_message>
HRMS Regression test script First Commit
</commit_message>
<xml_diff>
--- a/src/pom/Excel/TestCases/TestCases.xlsx
+++ b/src/pom/Excel/TestCases/TestCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="2">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -506,12 +506,6 @@
     <t>probation request should be submitted Successfully.</t>
   </si>
   <si>
-    <t>Probation Request send successfully</t>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
@@ -533,9 +527,6 @@
     <t>Porbation request should be  approve or reject successfully</t>
   </si>
   <si>
-    <t>Probation request approver or reject successfully</t>
-  </si>
-  <si>
     <t>26</t>
   </si>
   <si>
@@ -576,12 +567,6 @@
   </si>
   <si>
     <t>report should be generated successfully.</t>
-  </si>
-  <si>
-    <t>probation report not Generated Successfully</t>
-  </si>
-  <si>
-    <t>Failed</t>
   </si>
   <si>
     <t>28</t>
@@ -669,16 +654,339 @@
     <t>32</t>
   </si>
   <si>
+    <t>ELC</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>TC033_ResignationSubmition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of RM
+3) go to HRMS -&gt;  ELC -&gt; Exit -&gt; Resignation
+4) search Employee
+5) Edit Employee
+6) Submit Resignation Form
+9) observed.
+</t>
+  </si>
+  <si>
+    <t>Resignation should be submitted successfully.</t>
+  </si>
+  <si>
     <t>33</t>
   </si>
   <si>
+    <t>TC034_ResignationApprovarRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of RP
+3) go to HRMS -&gt;   ELC -&gt; Exit -&gt; Resignation Approvar by RP
+4) Search Employee.
+5) Edit Employee
+6)approve or reject by RP 
+10) observed.
+</t>
+  </si>
+  <si>
+    <t>Resignation should be approve or reject successfully by RP</t>
+  </si>
+  <si>
     <t>34</t>
   </si>
   <si>
-    <t>Probation Status showing properly</t>
-  </si>
-  <si>
-    <t>Basic Salary Added Successfully</t>
+    <t>TC035_ResignationApprovarHR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of HR
+3) go to HRMS -&gt;   ELC -&gt; Exit -&gt; Resignation Approvar by HR
+4) Search Employee.
+5) Edit Employee
+6)approve or reject by HR 
+10) observed.
+</t>
+  </si>
+  <si>
+    <t>Resignation should be approve or reject successfully by HR</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>TC036_ResignationStatusVerify</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of RM
+3) go to HRMS -&gt;  ELC -&gt; Exit -&gt; Resignation
+4) search Employee
+5) observed Status.
+</t>
+  </si>
+  <si>
+    <t>Resignation status should be showing  approved By HR</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>TC037_ExitForm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of Exit Employee's
+3) go to HRMS -&gt;  ELC -&gt; Exit -&gt; Exit Form
+4) fill all mandatory details and submit
+5) observed.
+</t>
+  </si>
+  <si>
+    <t>Exit Form should be submitted successfully.</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>TC038_ExitInterview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of HR
+3) go to HRMS -&gt;  ELC -&gt; Exit -&gt; Exit Interview
+4) fill all mandatory details and submit
+5) observed.
+</t>
+  </si>
+  <si>
+    <t>Exit Interview Form should be submited successfully</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>TC039_ExitInterviewEndorsement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of HR
+3) go to HRMS -&gt;  ELC -&gt; Exit -&gt; Exit Interview Endorsement
+4) fill all mandatory details and submit
+5) observed.
+</t>
+  </si>
+  <si>
+    <t>Exit Interview Endorsement Form should be submited successfully</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>TC040_LWDChange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid credentials of HR
+3) go to HRMS -&gt;  ELC -&gt; Exit -&gt; LWD Change
+4) search employee
+5) chnage LWD date and save.
+6) observed.
+</t>
+  </si>
+  <si>
+    <t>LWD should be change successfully.</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>TC041_AllowanceDeductionMasterDataUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid  admin credentials
+3) go to HRMS -&gt; HR Setup -&gt;  Rcruitment -&gt; allowance deduction master
+4)  click on add new button
+5) fill all mandatory details
+6) click on submit and observe
+</t>
+  </si>
+  <si>
+    <t>Allowance Deduction data should be added successfully</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>TC042_QualificationMasterDataUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid  admin credentials
+3) go to HRMS -&gt; HR Setup -&gt;  Rcruitment -&gt; qualification master
+4)  click on add new button
+5) fill all mandatory details
+6) click on submit and observe
+</t>
+  </si>
+  <si>
+    <t>qualification master data should be added successfully</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>TC043_CampusMasterDataUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid  admin credentials
+3) go to HRMS -&gt; HR Setup -&gt;  Rcruitment -&gt; Campus master
+4)  click on add new button
+5) fill all mandatory details
+7) click on submit and observe
+</t>
+  </si>
+  <si>
+    <t>Campus master data should be added successfully</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>TC044_ConsultantMasterDataUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid  admin credentials
+3) go to HRMS -&gt; HR Setup -&gt;  Rcruitment -&gt; Consultant master
+4)  click on add new button
+5) fill all mandatory details
+8) click on submit and observe
+</t>
+  </si>
+  <si>
+    <t>Consultant master data should be added successfully</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>TC045_FocusMasterDataUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid  admin credentials
+3) go to HRMS -&gt; HR Setup -&gt;  PMS and Training -&gt;Focus Master
+4)  click on add new button
+5) fill all mandatory details
+8) click on submit and observe
+</t>
+  </si>
+  <si>
+    <t>Focus master data should be added successfully</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>TC046_GoalMasterDataUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1)  open link 
+2) enter  valid  admin credentials
+3) go to HRMS -&gt; HR Setup -&gt;  PMS and Training -&gt;Goal Master
+4)  click on add new button
+5) fill all mandatory details
+9) click on submit and observe
+</t>
+  </si>
+  <si>
+    <t>Goal master data should be added successfully</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>Qualification Master record Added Successfully</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Focus Master record Added Successfully</t>
+  </si>
+  <si>
+    <t>Goal Master record Added Successfully</t>
   </si>
 </sst>
 </file>
@@ -838,7 +1146,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
@@ -865,13 +1173,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="2" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -880,10 +1189,6 @@
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="4" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="5" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
@@ -1233,8 +1538,8 @@
   <sheetPr/>
   <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
+      <selection activeCell="B47" sqref="B47:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1304,7 +1609,7 @@
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="18"/>
+      <c r="J2" s="17"/>
     </row>
     <row ht="120" r="3" spans="1:9">
       <c r="A3" s="6" t="s">
@@ -1403,8 +1708,8 @@
       <c r="G6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
     <row ht="150" r="7" spans="1:9">
       <c r="A7" s="6" t="s">
@@ -1528,8 +1833,8 @@
       <c r="G11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row ht="150" r="12" spans="1:9">
       <c r="A12" s="6" t="s">
@@ -1650,7 +1955,7 @@
       <c r="F16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>60</v>
       </c>
       <c r="H16" s="9"/>
@@ -1672,7 +1977,7 @@
       <c r="E17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>75</v>
       </c>
       <c r="G17" s="8" t="s">
@@ -1697,7 +2002,7 @@
       <c r="E18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>81</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -1722,7 +2027,7 @@
       <c r="E19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>85</v>
       </c>
       <c r="G19" s="8" t="s">
@@ -1747,7 +2052,7 @@
       <c r="E20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>90</v>
       </c>
       <c r="G20" s="8" t="s">
@@ -1772,14 +2077,14 @@
       <c r="E21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>95</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row ht="195" r="22" spans="1:9">
       <c r="A22" s="6" t="s">
@@ -1797,7 +2102,7 @@
       <c r="E22" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>102</v>
       </c>
       <c r="G22" s="8" t="s">
@@ -1822,14 +2127,14 @@
       <c r="E23" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>107</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
     </row>
     <row ht="150" r="24" spans="1:9">
       <c r="A24" s="6" t="s">
@@ -1847,14 +2152,14 @@
       <c r="E24" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>111</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
     </row>
     <row ht="180" r="25" spans="1:9">
       <c r="A25" s="6" t="s">
@@ -1872,633 +2177,946 @@
       <c r="E25" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>117</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H25" t="s">
-        <v>119</v>
-      </c>
-      <c r="I25" t="s">
-        <v>120</v>
-      </c>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
     </row>
     <row ht="180" r="26" spans="1:9">
       <c r="A26" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>124</v>
+      <c r="F26" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H26" t="s">
-        <v>126</v>
-      </c>
-      <c r="I26" t="s">
-        <v>120</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
     </row>
     <row ht="180" r="27" spans="1:9">
       <c r="A27" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>130</v>
+      <c r="F27" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="H27" t="s">
-        <v>126</v>
-      </c>
-      <c r="I27" t="s">
-        <v>120</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
     </row>
     <row ht="165" r="28" spans="1:9">
       <c r="A28" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>135</v>
+      <c r="F28" s="11" t="s">
+        <v>132</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H28" t="s">
-        <v>137</v>
-      </c>
-      <c r="I28" t="s">
-        <v>138</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
     </row>
     <row ht="180" r="29" spans="1:9">
       <c r="A29" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row ht="180" r="30" spans="1:9">
+      <c r="A30" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="B30" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="E30" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="15" t="s">
+      <c r="G30" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-    </row>
-    <row ht="180" r="30" spans="1:9">
-      <c r="A30" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
     </row>
     <row ht="180" r="31" spans="1:9">
       <c r="A31" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E31" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
+      <c r="F31" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
     </row>
     <row ht="180" r="32" spans="1:9">
       <c r="A32" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row ht="180" r="33" spans="1:9">
+      <c r="A33" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="13" t="s">
+      <c r="C33" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="D33" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="G32" s="11" t="s">
+      <c r="F33" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="H32" t="s">
-        <v>161</v>
-      </c>
-      <c r="I32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="6" t="s">
+      <c r="G33" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row ht="180" r="34" spans="1:9">
       <c r="A34" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="B34" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row ht="180" r="35" spans="1:9">
       <c r="A35" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>165</v>
+      </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-    </row>
-    <row r="38" spans="8:9">
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-    </row>
-    <row r="39" spans="8:9">
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-    </row>
-    <row r="40" spans="8:9">
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-    </row>
-    <row r="41" spans="8:9">
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-    </row>
-    <row r="42" spans="8:9">
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-    </row>
-    <row r="43" spans="8:9">
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-    </row>
-    <row r="44" spans="8:9">
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-    </row>
-    <row r="45" spans="8:9">
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="8:9">
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-    </row>
-    <row r="47" spans="8:9">
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-    </row>
-    <row r="48" spans="8:9">
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-    </row>
-    <row r="49" spans="8:9">
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-    </row>
-    <row r="50" spans="8:9">
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-    </row>
-    <row r="51" spans="8:9">
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-    </row>
-    <row r="52" spans="8:9">
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-    </row>
-    <row r="53" spans="8:9">
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-    </row>
-    <row r="54" spans="8:9">
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-    </row>
-    <row r="55" spans="8:9">
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-    </row>
-    <row r="56" spans="8:9">
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-    </row>
-    <row r="57" spans="8:9">
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-    </row>
-    <row r="58" spans="8:9">
-      <c r="H58" s="18"/>
-      <c r="I58" s="18"/>
-    </row>
-    <row r="59" spans="8:9">
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-    </row>
-    <row r="60" spans="8:9">
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-    </row>
-    <row r="61" spans="8:9">
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-    </row>
-    <row r="62" spans="8:9">
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-    </row>
-    <row r="63" spans="8:9">
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-    </row>
-    <row r="64" spans="8:9">
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-    </row>
-    <row r="65" spans="8:9">
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-    </row>
-    <row r="66" spans="8:9">
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
-    </row>
-    <row r="67" spans="8:9">
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-    </row>
-    <row r="68" spans="8:9">
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
+    <row ht="150" r="36" spans="1:9">
+      <c r="A36" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row ht="150" r="37" spans="1:9">
+      <c r="A37" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row ht="150" r="38" spans="1:9">
+      <c r="A38" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row ht="150" r="39" spans="1:9">
+      <c r="A39" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+    </row>
+    <row ht="165" r="40" spans="1:9">
+      <c r="A40" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+    </row>
+    <row ht="165" r="41" spans="1:9">
+      <c r="A41" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+    </row>
+    <row ht="165" r="42" spans="1:9">
+      <c r="A42" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row ht="165" r="43" spans="1:9">
+      <c r="A43" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+    </row>
+    <row ht="165" r="44" spans="1:9">
+      <c r="A44" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+    </row>
+    <row ht="165" r="45" spans="1:9">
+      <c r="A45" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="H45" t="s">
+        <v>235</v>
+      </c>
+      <c r="I45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row ht="165" r="46" spans="1:9">
+      <c r="A46" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="H46" t="s">
+        <v>236</v>
+      </c>
+      <c r="I46" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
     </row>
     <row r="69" spans="8:9">
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
     </row>
     <row r="70" spans="8:9">
-      <c r="H70" s="18"/>
-      <c r="I70" s="18"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
     </row>
     <row r="71" spans="8:9">
-      <c r="H71" s="18"/>
-      <c r="I71" s="18"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
     </row>
     <row r="72" spans="8:9">
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
     </row>
     <row r="73" spans="8:9">
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
     </row>
     <row r="74" spans="8:9">
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
     </row>
     <row r="75" spans="8:9">
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
     </row>
     <row r="76" spans="8:9">
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
     </row>
     <row r="77" spans="8:9">
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
     </row>
     <row r="78" spans="8:9">
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
     </row>
     <row r="79" spans="8:9">
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
     </row>
     <row r="80" spans="8:9">
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
     </row>
     <row r="81" spans="8:9">
-      <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
     </row>
     <row r="82" spans="8:9">
-      <c r="H82" s="18"/>
-      <c r="I82" s="18"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
     </row>
     <row r="83" spans="8:9">
-      <c r="H83" s="18"/>
-      <c r="I83" s="18"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
     </row>
     <row r="84" spans="8:9">
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
     </row>
     <row r="85" spans="8:9">
-      <c r="H85" s="18"/>
-      <c r="I85" s="18"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
     </row>
     <row r="86" spans="8:9">
-      <c r="H86" s="18"/>
-      <c r="I86" s="18"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
     </row>
     <row r="87" spans="8:9">
-      <c r="H87" s="18"/>
-      <c r="I87" s="18"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
     </row>
     <row r="88" spans="8:9">
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
     </row>
     <row r="89" spans="8:9">
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
     </row>
     <row r="90" spans="8:9">
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
     </row>
     <row r="91" spans="8:9">
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
     </row>
     <row r="92" spans="8:9">
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="17"/>
     </row>
     <row r="93" spans="8:9">
-      <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
     </row>
     <row r="94" spans="8:9">
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
     </row>
     <row r="95" spans="8:9">
-      <c r="H95" s="18"/>
-      <c r="I95" s="18"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
     </row>
     <row r="96" spans="8:9">
-      <c r="H96" s="18"/>
-      <c r="I96" s="18"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
     </row>
     <row r="97" spans="8:9">
-      <c r="H97" s="18"/>
-      <c r="I97" s="18"/>
+      <c r="H97" s="17"/>
+      <c r="I97" s="17"/>
     </row>
     <row r="98" spans="8:9">
-      <c r="H98" s="18"/>
-      <c r="I98" s="18"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
     </row>
     <row r="99" spans="8:9">
-      <c r="H99" s="18"/>
-      <c r="I99" s="18"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
     </row>
     <row r="100" spans="8:9">
-      <c r="H100" s="18"/>
-      <c r="I100" s="18"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
     </row>
     <row r="101" spans="8:9">
-      <c r="H101" s="18"/>
-      <c r="I101" s="18"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
     </row>
     <row r="102" spans="8:9">
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="17"/>
     </row>
     <row r="103" spans="8:9">
-      <c r="H103" s="18"/>
-      <c r="I103" s="18"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
     </row>
     <row r="104" spans="8:9">
-      <c r="H104" s="18"/>
-      <c r="I104" s="18"/>
+      <c r="H104" s="17"/>
+      <c r="I104" s="17"/>
     </row>
     <row r="105" spans="8:9">
-      <c r="H105" s="18"/>
-      <c r="I105" s="18"/>
+      <c r="H105" s="17"/>
+      <c r="I105" s="17"/>
     </row>
     <row r="106" spans="8:9">
-      <c r="H106" s="18"/>
-      <c r="I106" s="18"/>
+      <c r="H106" s="17"/>
+      <c r="I106" s="17"/>
     </row>
     <row r="107" spans="8:9">
-      <c r="H107" s="18"/>
-      <c r="I107" s="18"/>
+      <c r="H107" s="17"/>
+      <c r="I107" s="17"/>
     </row>
     <row r="108" spans="8:9">
-      <c r="H108" s="18"/>
-      <c r="I108" s="18"/>
+      <c r="H108" s="17"/>
+      <c r="I108" s="17"/>
     </row>
     <row r="109" spans="8:9">
-      <c r="H109" s="18"/>
-      <c r="I109" s="18"/>
+      <c r="H109" s="17"/>
+      <c r="I109" s="17"/>
     </row>
     <row r="110" spans="8:9">
-      <c r="H110" s="18"/>
-      <c r="I110" s="18"/>
+      <c r="H110" s="17"/>
+      <c r="I110" s="17"/>
     </row>
     <row r="111" spans="8:9">
-      <c r="H111" s="18"/>
-      <c r="I111" s="18"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="17"/>
     </row>
     <row r="112" spans="8:9">
-      <c r="H112" s="18"/>
-      <c r="I112" s="18"/>
+      <c r="H112" s="17"/>
+      <c r="I112" s="17"/>
     </row>
     <row r="113" spans="8:9">
-      <c r="H113" s="18"/>
-      <c r="I113" s="18"/>
+      <c r="H113" s="17"/>
+      <c r="I113" s="17"/>
     </row>
     <row r="114" spans="8:9">
-      <c r="H114" s="18"/>
-      <c r="I114" s="18"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="17"/>
     </row>
     <row r="115" spans="8:9">
-      <c r="H115" s="18"/>
-      <c r="I115" s="18"/>
+      <c r="H115" s="17"/>
+      <c r="I115" s="17"/>
     </row>
     <row r="116" spans="8:9">
-      <c r="H116" s="18"/>
-      <c r="I116" s="18"/>
+      <c r="H116" s="17"/>
+      <c r="I116" s="17"/>
     </row>
     <row r="117" spans="8:9">
-      <c r="H117" s="18"/>
-      <c r="I117" s="18"/>
+      <c r="H117" s="17"/>
+      <c r="I117" s="17"/>
     </row>
     <row r="118" spans="8:9">
-      <c r="H118" s="18"/>
-      <c r="I118" s="18"/>
+      <c r="H118" s="17"/>
+      <c r="I118" s="17"/>
     </row>
     <row r="119" spans="8:9">
-      <c r="H119" s="18"/>
-      <c r="I119" s="18"/>
+      <c r="H119" s="17"/>
+      <c r="I119" s="17"/>
     </row>
     <row r="120" spans="8:9">
-      <c r="H120" s="18"/>
-      <c r="I120" s="18"/>
+      <c r="H120" s="17"/>
+      <c r="I120" s="17"/>
     </row>
     <row r="121" spans="8:9">
-      <c r="H121" s="18"/>
-      <c r="I121" s="18"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="17"/>
     </row>
     <row r="122" spans="8:9">
-      <c r="H122" s="18"/>
-      <c r="I122" s="18"/>
+      <c r="H122" s="17"/>
+      <c r="I122" s="17"/>
     </row>
     <row r="123" spans="8:9">
-      <c r="H123" s="18"/>
-      <c r="I123" s="18"/>
+      <c r="H123" s="17"/>
+      <c r="I123" s="17"/>
     </row>
     <row r="124" spans="8:9">
-      <c r="H124" s="18"/>
-      <c r="I124" s="18"/>
+      <c r="H124" s="17"/>
+      <c r="I124" s="17"/>
     </row>
     <row r="125" spans="8:9">
-      <c r="H125" s="18"/>
-      <c r="I125" s="18"/>
+      <c r="H125" s="17"/>
+      <c r="I125" s="17"/>
     </row>
     <row r="126" spans="8:9">
-      <c r="H126" s="18"/>
-      <c r="I126" s="18"/>
+      <c r="H126" s="17"/>
+      <c r="I126" s="17"/>
     </row>
     <row r="127" spans="8:9">
       <c r="H127" t="s">
-        <v>160</v>
+        <v>233</v>
       </c>
       <c r="I127" t="s">
-        <v>120</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>